<commit_message>
abstracted methods in homepage
</commit_message>
<xml_diff>
--- a/src/test/resources/MetTestCases.xlsx
+++ b/src/test/resources/MetTestCases.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabreenmostafa/IdeaProjects/METModule/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF03331B-4497-4845-8E39-5451A56B072C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D47D06-17E3-AF49-A90E-722D737D93E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="700" windowWidth="27340" windowHeight="16940" activeTab="2" xr2:uid="{569C5C2E-E302-A143-B341-2BF8C097B459}"/>
+    <workbookView xWindow="1460" yWindow="500" windowWidth="27340" windowHeight="16940" activeTab="4" xr2:uid="{569C5C2E-E302-A143-B341-2BF8C097B459}"/>
   </bookViews>
   <sheets>
     <sheet name="MetSRT1" sheetId="1" r:id="rId1"/>
     <sheet name="MetStoreT1" sheetId="2" r:id="rId2"/>
     <sheet name="Exhibitions" sheetId="3" r:id="rId3"/>
+    <sheet name="Explore" sheetId="5" r:id="rId4"/>
+    <sheet name="Rules" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>SUNFLOWERS</t>
   </si>
@@ -212,9 +214,6 @@
     <t>In Praise of Painting: Dutch Masterpieces at The Met</t>
   </si>
   <si>
-    <t>Spain, 1000–1200: Art at the Frontiers of Faith</t>
-  </si>
-  <si>
     <t>Japan: A History of Style</t>
   </si>
   <si>
@@ -261,6 +260,63 @@
   </si>
   <si>
     <t>Fabergé from the Matilda Geddings Gray Foundation Collection</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/perspectives</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/150</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/art/object-package?pkgids=725</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/join-and-give/travel-with-the-met</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/events/programs/virtual-events</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/learn</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/art/metpublications</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/visit/group-visits</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/visit/audio-content</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/about-the-met/conservation-and-scientific-research</t>
+  </si>
+  <si>
+    <t>https://www.metmuseum.org/about-the-met/collection-areas</t>
+  </si>
+  <si>
+    <t>Face coverings are required for all visitors age two and older, even if you are vaccinated.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintain physical distancing. Keep at least six feet from others. </t>
+  </si>
+  <si>
+    <t>Report symptoms of illness.</t>
+  </si>
+  <si>
+    <t>Wash hands and use hand sanitizer regularly during your visit.</t>
+  </si>
+  <si>
+    <t>Select food and beverage options are available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coat check is temporarily closed. No large bags. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please follow directions from Met staff. </t>
+  </si>
+  <si>
+    <t>Please do not touch the art.</t>
   </si>
 </sst>
 </file>
@@ -897,10 +953,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8464228-1B70-AF4E-BFC0-9797E71E618D}">
-  <dimension ref="A2:A25"/>
+  <dimension ref="A2:A24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1020,9 +1076,129 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90EF3D6-7B00-2C4B-99B9-CFB666954E41}">
+  <dimension ref="A2:A12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF75BC14-0EF8-3A4D-BA58-357D75059B51}">
+  <dimension ref="A2:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>